<commit_message>
working updated tree and database schema
</commit_message>
<xml_diff>
--- a/output/assets/laptop_invoices_download.xlsx
+++ b/output/assets/laptop_invoices_download.xlsx
@@ -533,37 +533,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HYD8-1345061</t>
+          <t>FAAOZK2200001887</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>02-04-2021</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>04-04-2021</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>403-0151201-6865928</t>
+          <t>OD121420552428604000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CLICKTECH RETAIL PRIVATE LIMITED</t>
+          <t>Sane Retails Private Limited</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Apple MacBook Air Laptop M1 chip, 13.3-inch/33.74 cm Retina Display, 8GB RAM, 256GB SSD Storage, Backlit Keyboard, FaceTime HD Camera, Touch ID. Works with iPhone/iPad; Space Grey | B08N5W4NNB</t>
+          <t>MacBook Air</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>i5 5th Gen</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -573,37 +573,27 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>256GB SSD</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Space Grey</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>13.3-inch</t>
-        </is>
-      </c>
+          <t>128GB SSD</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+          <t>Mac OS Sierra</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>s12345</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
+          <t>SFVFDL811J1WK</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>12</v>
+      </c>
       <c r="P2" t="n">
-        <v>44906.78</v>
+        <v>67640</v>
       </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
@@ -639,7 +629,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Apple MacBook Air Laptop M1 chip, 13.3-inch/33.74 cm Retina Display, 8GB RAM, 256GB SSD Storage, Backlit Keyboard, FaceTime HD Camera, Touch ID. Works with iPhone/iPad; Space Grey | B08N5W4NNB</t>
+          <t>MacBook Air</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -708,7 +698,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Apple MacBook Air Laptop M1 chip, 13.3-inch/33.74 cm Retina Display, 8GB RAM, 256GB SSD Storage, Backlit Keyboard, FaceTime HD Camera, Touch ID. Works with iPhone/iPad; Space Grey | B08N5W4NNB</t>
+          <t>MacBook Air</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -777,7 +767,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Apple MacBook Air Laptop M1 chip, 13.3-inch/33.74 cm Retina Display, 8GB RAM, 256GB SSD Storage, Backlit Keyboard, FaceTime HD Camera, Touch ID. Works with iPhone/iPad; Space Grey | B08N5W4NNB</t>
+          <t>MacBook Air</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -821,67 +811,65 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FAAOZK2200001887</t>
+          <t>HYD8-1345061</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02-04-2021</t>
+          <t>26-09-2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>04-04-2021</t>
+          <t>26-09-2024</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>OD121420552428604000</t>
+          <t>403-0151201-6865928</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sane Retails Private Limited</t>
+          <t>CLICKTECH RETAIL PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>APPLE MacBook Air Core i5 5th Gen - (8 GB/128 GB SSD/Mac OS Sierra) MQD32HN/A</t>
+          <t>MacBook Air</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>i5 5th Gen</t>
+          <t>M1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>8 GB</t>
+          <t>8GB</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>128 GB SSD</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Mac OS Sierra</t>
-        </is>
-      </c>
+          <t>256GB SSD</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Space Grey</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>13.3-inch</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>SFVFDL811 J1WK</t>
-        </is>
-      </c>
-      <c r="O6" t="n">
-        <v>12</v>
-      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
-        <v>67640</v>
+        <v>44906.78</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>

</xml_diff>